<commit_message>
bump buffer version to 0.2
</commit_message>
<xml_diff>
--- a/development/arena_12-12/teensy4p1/teensy_arena_12-12_v0p1/production/version_0p1_r1/nonlscs_bom_teensy_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12/teensy4p1/teensy_arena_12-12_v0p1/production/version_0p1_r1/nonlscs_bom_teensy_arena_12-12_v0p1_r1.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">DC Power Barrel Jack</t>
   </si>
   <si>
-    <t xml:space="preserve">J1, J4</t>
+    <t xml:space="preserve">J1</t>
   </si>
   <si>
     <t xml:space="preserve">through hole</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Teensy 4.1</t>
   </si>
   <si>
-    <t xml:space="preserve">U1</t>
+    <t xml:space="preserve">U18</t>
   </si>
   <si>
     <t xml:space="preserve">1568-DEV-16771-ND</t>
@@ -205,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +232,14 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -319,10 +327,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,28 +345,32 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="10.41"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
       <c r="D1" s="5"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -373,7 +385,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -419,22 +431,22 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -475,10 +487,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>